<commit_message>
Added Country Report #147
</commit_message>
<xml_diff>
--- a/app/data/publicationsList.xlsx
+++ b/app/data/publicationsList.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kannanvenkat/Documents/worldBank/CLAIR/Dashboard/institutional-assessment-dashboard/app/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768B31F8-4769-2245-AD6C-C25EE120E1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>title</t>
   </si>
@@ -66,33 +75,66 @@
   <si>
     <t>https://documents.worldbank.org/en/publication/documents-reports/documentdetail/596001618377875403/climate-change-institutional-assessment</t>
   </si>
+  <si>
+    <t>Country Report</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1QFwFRmB5Mu9KOgp5PZNtsVG3gtfJS_Xu/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>publications/CR_Uruguay.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,42 +142,49 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -325,26 +374,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.88"/>
-    <col customWidth="1" min="3" max="3" width="16.38"/>
-    <col customWidth="1" min="4" max="4" width="23.0"/>
-    <col customWidth="1" min="5" max="5" width="28.0"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -364,7 +418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -372,7 +426,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="2">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -384,7 +438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -392,7 +446,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
@@ -402,13 +456,34 @@
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" location=":~:text=Croatia-,Croatia%20Country%20Economic%20Memorandum%20%3A%20Laying%20the%20Foundations%20%2D%20Boosting%20Productivity%20to,and%20productivity%20of%20its%20economy." ref="F2"/>
-    <hyperlink r:id="rId2" ref="F3"/>
+    <hyperlink ref="F2" r:id="rId1" location=":~:text=Croatia-,Croatia%20Country%20Economic%20Memorandum%20%3A%20Laying%20the%20Foundations%20%2D%20Boosting%20Productivity%20to,and%20productivity%20of%20its%20economy." xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{4A8F1BB7-327A-434C-A416-3056DDCDFD24}"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added CCDR report #284
</commit_message>
<xml_diff>
--- a/app/data/publicationsList.xlsx
+++ b/app/data/publicationsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kannanvenkat/Documents/worldBank/CLAIR/Dashboard/institutional-assessment-dashboard/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664C1BB0-F554-7B43-A325-19AD7C7D37E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655440BA-5568-AD43-85AE-2B6D121D29CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>title</t>
   </si>
@@ -87,12 +87,27 @@
   <si>
     <t>publications/IA-UY-final-ENGLISH.pdf</t>
   </si>
+  <si>
+    <t>Country Climate and Development Report (CCDR)</t>
+  </si>
+  <si>
+    <t>publications/DRC CCDR Report.pdf</t>
+  </si>
+  <si>
+    <t>World Bank Group</t>
+  </si>
+  <si>
+    <t>Congo, Dem. Rep.</t>
+  </si>
+  <si>
+    <t>publications/DRC CCDR Report.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -122,14 +137,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -154,20 +161,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,10 +389,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -395,7 +400,7 @@
     <col min="1" max="1" width="36.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -478,11 +483,30 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>2023</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location=":~:text=Croatia-,Croatia%20Country%20Economic%20Memorandum%20%3A%20Laying%20the%20Foundations%20%2D%20Boosting%20Productivity%20to,and%20productivity%20of%20its%20economy." xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" display="https://drive.google.com/file/d/1QFwFRmB5Mu9KOgp5PZNtsVG3gtfJS_Xu/view?usp=drive_link" xr:uid="{4A8F1BB7-327A-434C-A416-3056DDCDFD24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>